<commit_message>
fixed bugs in VAR and arima
</commit_message>
<xml_diff>
--- a/Result/ARIMA/Manufacturing/AUS.xlsx
+++ b/Result/ARIMA/Manufacturing/AUS.xlsx
@@ -463,7 +463,7 @@
         <v>1990</v>
       </c>
       <c r="B2" t="n">
-        <v>13.79344438155173</v>
+        <v>-0.2964594439589135</v>
       </c>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr"/>
@@ -473,7 +473,7 @@
         <v>1991</v>
       </c>
       <c r="B3" t="n">
-        <v>12.5698102029463</v>
+        <v>13.49698493759282</v>
       </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr"/>
@@ -483,7 +483,7 @@
         <v>1992</v>
       </c>
       <c r="B4" t="n">
-        <v>12.58015887642892</v>
+        <v>12.27335075898739</v>
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr"/>
@@ -493,7 +493,7 @@
         <v>1993</v>
       </c>
       <c r="B5" t="n">
-        <v>12.87318388719052</v>
+        <v>12.28369943247001</v>
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr"/>
@@ -503,7 +503,7 @@
         <v>1994</v>
       </c>
       <c r="B6" t="n">
-        <v>13.20501995208072</v>
+        <v>12.57672444323161</v>
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr"/>
@@ -513,7 +513,7 @@
         <v>1995</v>
       </c>
       <c r="B7" t="n">
-        <v>13.12367686560688</v>
+        <v>12.90856050812181</v>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
@@ -523,7 +523,7 @@
         <v>1996</v>
       </c>
       <c r="B8" t="n">
-        <v>12.7424163318427</v>
+        <v>12.82721742164797</v>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
@@ -533,7 +533,7 @@
         <v>1997</v>
       </c>
       <c r="B9" t="n">
-        <v>12.30366539207597</v>
+        <v>12.44595688788379</v>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr"/>
@@ -543,7 +543,7 @@
         <v>1998</v>
       </c>
       <c r="B10" t="n">
-        <v>12.47074767085228</v>
+        <v>12.00720594811706</v>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr"/>
@@ -553,7 +553,7 @@
         <v>1999</v>
       </c>
       <c r="B11" t="n">
-        <v>11.95283158647435</v>
+        <v>12.17428822689337</v>
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr"/>
@@ -563,7 +563,7 @@
         <v>2000</v>
       </c>
       <c r="B12" t="n">
-        <v>11.57011554701219</v>
+        <v>11.65637214251544</v>
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr"/>
@@ -573,7 +573,7 @@
         <v>2001</v>
       </c>
       <c r="B13" t="n">
-        <v>10.99301372481012</v>
+        <v>11.27365610305328</v>
       </c>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr"/>
@@ -583,7 +583,7 @@
         <v>2002</v>
       </c>
       <c r="B14" t="n">
-        <v>10.55534894431952</v>
+        <v>10.69655428085121</v>
       </c>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
@@ -593,7 +593,7 @@
         <v>2003</v>
       </c>
       <c r="B15" t="n">
-        <v>10.86216994180758</v>
+        <v>10.25888950036061</v>
       </c>
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr"/>
@@ -603,7 +603,7 @@
         <v>2004</v>
       </c>
       <c r="B16" t="n">
-        <v>10.88215706600108</v>
+        <v>10.56571049784867</v>
       </c>
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr"/>
@@ -613,7 +613,7 @@
         <v>2005</v>
       </c>
       <c r="B17" t="n">
-        <v>10.33486230097914</v>
+        <v>10.58569762204217</v>
       </c>
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr"/>
@@ -623,7 +623,7 @@
         <v>2006</v>
       </c>
       <c r="B18" t="n">
-        <v>9.892071199355792</v>
+        <v>10.03840285702023</v>
       </c>
       <c r="C18" t="inlineStr"/>
       <c r="D18" t="inlineStr"/>
@@ -633,7 +633,7 @@
         <v>2007</v>
       </c>
       <c r="B19" t="n">
-        <v>9.290666490144647</v>
+        <v>9.595611755396879</v>
       </c>
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="inlineStr"/>
@@ -643,7 +643,7 @@
         <v>2008</v>
       </c>
       <c r="B20" t="n">
-        <v>9.202198922938425</v>
+        <v>8.994207046185732</v>
       </c>
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr"/>
@@ -653,7 +653,7 @@
         <v>2009</v>
       </c>
       <c r="B21" t="n">
-        <v>8.453526785289274</v>
+        <v>8.905739478979513</v>
       </c>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr"/>
@@ -663,7 +663,7 @@
         <v>2010</v>
       </c>
       <c r="B22" t="n">
-        <v>7.997034212477491</v>
+        <v>8.157067341330361</v>
       </c>
       <c r="C22" t="inlineStr"/>
       <c r="D22" t="inlineStr"/>
@@ -673,7 +673,7 @@
         <v>2011</v>
       </c>
       <c r="B23" t="n">
-        <v>7.368513108841397</v>
+        <v>7.700574768518576</v>
       </c>
       <c r="C23" t="inlineStr"/>
       <c r="D23" t="inlineStr"/>
@@ -683,7 +683,7 @@
         <v>2012</v>
       </c>
       <c r="B24" t="n">
-        <v>7.05045459273345</v>
+        <v>7.072053664882484</v>
       </c>
       <c r="C24" t="inlineStr"/>
       <c r="D24" t="inlineStr"/>
@@ -693,7 +693,7 @@
         <v>2013</v>
       </c>
       <c r="B25" t="n">
-        <v>6.608333214010963</v>
+        <v>6.753995148774536</v>
       </c>
       <c r="C25" t="inlineStr"/>
       <c r="D25" t="inlineStr"/>
@@ -703,7 +703,7 @@
         <v>2014</v>
       </c>
       <c r="B26" t="n">
-        <v>6.368634633947076</v>
+        <v>6.311873770052049</v>
       </c>
       <c r="C26" t="inlineStr"/>
       <c r="D26" t="inlineStr"/>
@@ -713,7 +713,7 @@
         <v>2015</v>
       </c>
       <c r="B27" t="n">
-        <v>6.299997474136078</v>
+        <v>6.072175189988163</v>
       </c>
       <c r="C27" t="inlineStr"/>
       <c r="D27" t="inlineStr"/>
@@ -723,7 +723,7 @@
         <v>2016</v>
       </c>
       <c r="B28" t="n">
-        <v>6.085499329208853</v>
+        <v>6.003538030177165</v>
       </c>
       <c r="C28" t="inlineStr"/>
       <c r="D28" t="inlineStr"/>
@@ -885,7 +885,7 @@
         <v>1990</v>
       </c>
       <c r="B2" t="n">
-        <v>13.79344438155173</v>
+        <v>-0.2654151558693363</v>
       </c>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr"/>
@@ -895,7 +895,7 @@
         <v>1991</v>
       </c>
       <c r="B3" t="n">
-        <v>12.5698102029463</v>
+        <v>13.52802922568239</v>
       </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr"/>
@@ -905,7 +905,7 @@
         <v>1992</v>
       </c>
       <c r="B4" t="n">
-        <v>12.58015887642892</v>
+        <v>12.30439504707696</v>
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr"/>
@@ -915,7 +915,7 @@
         <v>1993</v>
       </c>
       <c r="B5" t="n">
-        <v>12.87318388719052</v>
+        <v>12.31474372055958</v>
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr"/>
@@ -925,7 +925,7 @@
         <v>1994</v>
       </c>
       <c r="B6" t="n">
-        <v>13.20501995208072</v>
+        <v>12.60776873132118</v>
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr"/>
@@ -935,7 +935,7 @@
         <v>1995</v>
       </c>
       <c r="B7" t="n">
-        <v>13.12367686560688</v>
+        <v>12.93960479621138</v>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
@@ -945,7 +945,7 @@
         <v>1996</v>
       </c>
       <c r="B8" t="n">
-        <v>12.7424163318427</v>
+        <v>12.85826170973754</v>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
@@ -955,7 +955,7 @@
         <v>1997</v>
       </c>
       <c r="B9" t="n">
-        <v>12.30366539207597</v>
+        <v>12.47700117597336</v>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr"/>
@@ -965,7 +965,7 @@
         <v>1998</v>
       </c>
       <c r="B10" t="n">
-        <v>12.47074767085228</v>
+        <v>12.03825023620663</v>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr"/>
@@ -975,7 +975,7 @@
         <v>1999</v>
       </c>
       <c r="B11" t="n">
-        <v>11.95283158647435</v>
+        <v>12.20533251498294</v>
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr"/>
@@ -985,7 +985,7 @@
         <v>2000</v>
       </c>
       <c r="B12" t="n">
-        <v>11.57011554701219</v>
+        <v>11.68741643060501</v>
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr"/>
@@ -995,7 +995,7 @@
         <v>2001</v>
       </c>
       <c r="B13" t="n">
-        <v>10.99301372481012</v>
+        <v>11.30470039114285</v>
       </c>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr"/>
@@ -1005,7 +1005,7 @@
         <v>2002</v>
       </c>
       <c r="B14" t="n">
-        <v>10.55534894431952</v>
+        <v>10.72759856894078</v>
       </c>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
@@ -1015,7 +1015,7 @@
         <v>2003</v>
       </c>
       <c r="B15" t="n">
-        <v>10.86216994180758</v>
+        <v>10.28993378845018</v>
       </c>
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr"/>
@@ -1025,7 +1025,7 @@
         <v>2004</v>
       </c>
       <c r="B16" t="n">
-        <v>10.88215706600108</v>
+        <v>10.59675478593824</v>
       </c>
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr"/>
@@ -1035,7 +1035,7 @@
         <v>2005</v>
       </c>
       <c r="B17" t="n">
-        <v>10.33486230097914</v>
+        <v>10.61674191013174</v>
       </c>
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr"/>
@@ -1045,7 +1045,7 @@
         <v>2006</v>
       </c>
       <c r="B18" t="n">
-        <v>9.892071199355792</v>
+        <v>10.0694471451098</v>
       </c>
       <c r="C18" t="inlineStr"/>
       <c r="D18" t="inlineStr"/>
@@ -1055,7 +1055,7 @@
         <v>2007</v>
       </c>
       <c r="B19" t="n">
-        <v>9.290666490144647</v>
+        <v>9.626656043486456</v>
       </c>
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="inlineStr"/>
@@ -1065,7 +1065,7 @@
         <v>2008</v>
       </c>
       <c r="B20" t="n">
-        <v>9.202198922938425</v>
+        <v>9.02525133427531</v>
       </c>
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr"/>
@@ -1075,7 +1075,7 @@
         <v>2009</v>
       </c>
       <c r="B21" t="n">
-        <v>8.453526785289274</v>
+        <v>8.936783767069089</v>
       </c>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr"/>
@@ -1085,7 +1085,7 @@
         <v>2010</v>
       </c>
       <c r="B22" t="n">
-        <v>7.997034212477491</v>
+        <v>8.188111629419938</v>
       </c>
       <c r="C22" t="inlineStr"/>
       <c r="D22" t="inlineStr"/>
@@ -1095,7 +1095,7 @@
         <v>2011</v>
       </c>
       <c r="B23" t="n">
-        <v>7.368513108841397</v>
+        <v>7.731619056608155</v>
       </c>
       <c r="C23" t="inlineStr"/>
       <c r="D23" t="inlineStr"/>
@@ -1105,7 +1105,7 @@
         <v>2012</v>
       </c>
       <c r="B24" t="n">
-        <v>7.05045459273345</v>
+        <v>7.103097952972061</v>
       </c>
       <c r="C24" t="inlineStr"/>
       <c r="D24" t="inlineStr"/>
@@ -1115,7 +1115,7 @@
         <v>2013</v>
       </c>
       <c r="B25" t="n">
-        <v>6.608333214010963</v>
+        <v>6.785039436864114</v>
       </c>
       <c r="C25" t="inlineStr"/>
       <c r="D25" t="inlineStr"/>
@@ -1125,7 +1125,7 @@
         <v>2014</v>
       </c>
       <c r="B26" t="n">
-        <v>6.368634633947076</v>
+        <v>6.342918058141627</v>
       </c>
       <c r="C26" t="inlineStr"/>
       <c r="D26" t="inlineStr"/>
@@ -1135,7 +1135,7 @@
         <v>2015</v>
       </c>
       <c r="B27" t="n">
-        <v>6.299997474136078</v>
+        <v>6.10321947807774</v>
       </c>
       <c r="C27" t="inlineStr"/>
       <c r="D27" t="inlineStr"/>
@@ -1145,7 +1145,7 @@
         <v>2016</v>
       </c>
       <c r="B28" t="n">
-        <v>6.085499329208853</v>
+        <v>6.034582318266742</v>
       </c>
       <c r="C28" t="inlineStr"/>
       <c r="D28" t="inlineStr"/>
@@ -1155,7 +1155,7 @@
         <v>2017</v>
       </c>
       <c r="B29" t="n">
-        <v>5.798737462442747</v>
+        <v>5.820084173339517</v>
       </c>
       <c r="C29" t="inlineStr"/>
       <c r="D29" t="inlineStr"/>
@@ -1165,7 +1165,7 @@
         <v>2018</v>
       </c>
       <c r="B30" t="n">
-        <v>5.777271824567839</v>
+        <v>5.533322306573411</v>
       </c>
       <c r="C30" t="inlineStr"/>
       <c r="D30" t="inlineStr"/>
@@ -1175,7 +1175,7 @@
         <v>2019</v>
       </c>
       <c r="B31" t="n">
-        <v>5.615118064276127</v>
+        <v>5.511856668698503</v>
       </c>
       <c r="C31" t="inlineStr"/>
       <c r="D31" t="inlineStr"/>
@@ -1185,7 +1185,7 @@
         <v>2020</v>
       </c>
       <c r="B32" t="n">
-        <v>5.651114209643661</v>
+        <v>5.349702908406791</v>
       </c>
       <c r="C32" t="inlineStr"/>
       <c r="D32" t="inlineStr"/>
@@ -1195,7 +1195,7 @@
         <v>2021</v>
       </c>
       <c r="B33" t="n">
-        <v>5.565623775405053</v>
+        <v>5.385699053774325</v>
       </c>
       <c r="C33" t="inlineStr"/>
       <c r="D33" t="inlineStr"/>

</xml_diff>